<commit_message>
Housekeeping (move files to new directory structure)
</commit_message>
<xml_diff>
--- a/pipelinetable.xlsx
+++ b/pipelinetable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="141">
   <si>
     <t>Path to script</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Spatial data processing</t>
   </si>
   <si>
-    <t>NLCD/cliptncusa.R</t>
-  </si>
-  <si>
     <t>/nfs/qread-data/raw_data/landuse/ecoregions/tnc_terr_ecoregions.shp; /nfs/public-data/GADM/USA_adm/USA_adm0.shp</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Creating maps and visualizations</t>
   </si>
   <si>
-    <t>FAF/cfs_tnc_intersect.sh</t>
-  </si>
-  <si>
     <t>fwe/read_data/transform_cfs.sh</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>Albers TNC ecoregion shapefile and USA shapefile</t>
   </si>
   <si>
-    <t>FAF/fix_map_codes.R</t>
-  </si>
-  <si>
     <t>CFS Albers shapefile, FAF lookup table made elsewhere</t>
   </si>
   <si>
@@ -239,9 +230,6 @@
     <t>land exchanges from satellite tables in R-readable form, recategorized into Chaudhary's categories</t>
   </si>
   <si>
-    <t>FAF/faf_bea_viz.R</t>
-  </si>
-  <si>
     <t>FAF by BEA object; CFS Albers GPKG; FAF lookup table; NAICS/BEA/SCTG crosswalk</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>qread-data/figures/fafmaps/inflows or outflows or netflows _ cropland or pastureland.png</t>
   </si>
   <si>
-    <t>The first 80 lines of this script are "sourced" in other scripts</t>
-  </si>
-  <si>
     <t>FAF/impute_exchanges.R</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t>faf_eeio_output_full.Rdata</t>
   </si>
   <si>
-    <t>FAF/map_eeio_faf.R</t>
-  </si>
-  <si>
     <t>CFS Albers shapefile; FAF lookup table; FAF EEIO impacts full object</t>
   </si>
   <si>
@@ -386,9 +368,6 @@
     <t>maps/nettransfer_prelim…png</t>
   </si>
   <si>
-    <t>FAF/tnc_land_transfer_maps.R</t>
-  </si>
-  <si>
     <t>jobscripts/sbatch_calls.sh</t>
   </si>
   <si>
@@ -401,12 +380,6 @@
     <t>FAF/faf_land_transfer_to_tnc.R</t>
   </si>
   <si>
-    <t>Same inputs as faf_land_transfers.R, and additionally NLCD tabulated by the CFS-TNC intersect</t>
-  </si>
-  <si>
-    <t>faf_by_bea.Rdata; faf_region_lookup.csv; nass_bea_state_x_faf_land_totals.csv; raw_data/landuse/output_csvs/NLCD_2016_CFSTNC.csv</t>
-  </si>
-  <si>
     <t>NLCD cropland and pastureland totals by CFS-TNC intersect; FAF by BEA object modified with all cropland and pastureland flows; exiting flows of cropland and pastureland from TNC regions to FAF regions</t>
   </si>
   <si>
@@ -435,6 +408,45 @@
   </si>
   <si>
     <t>maps/tnc_outgoing_crop or pasture.png</t>
+  </si>
+  <si>
+    <t>Sourced in other scripts</t>
+  </si>
+  <si>
+    <t>figs/faf_land_transfer_maps.R</t>
+  </si>
+  <si>
+    <t>none (begins by sourcing faf_land_transfers.R)</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>none (intermediate, produces objects in R workspace)</t>
+  </si>
+  <si>
+    <t>begins by sourcing faf_land_transfers.R, and additionally NLCD tabulated by the CFS-TNC intersect</t>
+  </si>
+  <si>
+    <t>raw_data/landuse/output_csvs/NLCD_2016_CFSTNC.csv</t>
+  </si>
+  <si>
+    <t>spatial_processing/cliptncusa.R</t>
+  </si>
+  <si>
+    <t>spatial_processing/fix_map_codes.R</t>
+  </si>
+  <si>
+    <t>spatial_processing/cfs_tnc_intersect.sh</t>
+  </si>
+  <si>
+    <t>figs/faf_bea_viz.R</t>
+  </si>
+  <si>
+    <t>figs/tnc_land_transfer_maps.R</t>
+  </si>
+  <si>
+    <t>figs/map_eeio_faf.R</t>
   </si>
 </sst>
 </file>
@@ -755,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,19 +812,19 @@
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -820,19 +832,19 @@
         <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -840,19 +852,19 @@
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -860,19 +872,19 @@
         <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -880,19 +892,19 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -900,16 +912,16 @@
         <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -920,47 +932,107 @@
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -969,376 +1041,336 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F27" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update pipeline with the foreign transfer information
</commit_message>
<xml_diff>
--- a/pipelinetable.xlsx
+++ b/pipelinetable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="186">
   <si>
     <t>Path to script</t>
   </si>
@@ -356,12 +356,6 @@
     <t>jobscripts/sbatch_calls.sh</t>
   </si>
   <si>
-    <t>NLCD 2016 tabulated by each of the shapefiles; Historic 1700 landcover tabulated by each of the shapefiles; CDL tabulated by each of the shapefiles; rasterized TNC tabulated by CFS and by state; rasterized BCR tabulated by CFS and by state</t>
-  </si>
-  <si>
-    <t>NLCD 2016 raster; historic 1700 land cover raster; CDL raster; rasterized TNC and BCR (Created elsewhere)</t>
-  </si>
-  <si>
     <t>FAF/faf_land_transfer_to_tnc.R</t>
   </si>
   <si>
@@ -404,12 +398,6 @@
     <t>none (intermediate, produces objects in R workspace)</t>
   </si>
   <si>
-    <t>begins by sourcing faf_land_transfers.R, and additionally NLCD tabulated by the CFS-TNC intersect</t>
-  </si>
-  <si>
-    <t>raw_data/landuse/output_csvs/NLCD_2016_CFSTNC.csv</t>
-  </si>
-  <si>
     <t>spatial_processing/cliptncusa.R</t>
   </si>
   <si>
@@ -431,12 +419,6 @@
     <t>Other than that does not download anything directly, should be done in parallel. Note: all comtrade data was moved to raw_data/commodity_flows/Comtrade/ on 21 Aug</t>
   </si>
   <si>
-    <t>Intermediate outputs: NLCD cropland and pastureland totals by CFS-TNC intersect; FAF by BEA object modified with all cropland and pastureland flows; exiting flows of cropland and pastureland from TNC regions to FAF regions. Additional outputs: TNC x TNC x FAF x FAF flows (all combinations) of land, and TNC x TNC aggregated flows</t>
-  </si>
-  <si>
-    <t>NLCDcrop_FAF_x_TNC.csv; FAF_all_flows_x_BEA.csv; FAF_all_flows_x_TNC.csv; FAF_all_flows_TNC_x_TNC.csv; TNC_x_TNC_all_flows.csv</t>
-  </si>
-  <si>
     <t>figs/tnc_flows_vis.R</t>
   </si>
   <si>
@@ -522,6 +504,84 @@
   </si>
   <si>
     <t>Summary visualizations of which ports receive the most virtual land and which regions get the most as imports</t>
+  </si>
+  <si>
+    <t>spatial_processing/transform_tnc_countries.sh</t>
+  </si>
+  <si>
+    <t>Global TNC shapefile, global country boundaries shapefile, global cropland and pasture rasters</t>
+  </si>
+  <si>
+    <t>all in raw_data/landuse/ecoregions: tnc_terr_ecoregions.shp, ne_50m_admin_0_countries.shp; pasture.tif; GFSAD*.tif</t>
+  </si>
+  <si>
+    <t>All the above converted to Mollweide projection</t>
+  </si>
+  <si>
+    <t>tnc_global_equalarea.gpkg; countries_global_equalarea.gpkg; pasture_equalarea.vrt; cropdominance_equalarea.vrt; cropmask_equalarea.vrt</t>
+  </si>
+  <si>
+    <t>spatial_processing/summarizepasture.py</t>
+  </si>
+  <si>
+    <t>Intersected CFS/TNC GPKG, pasture raster</t>
+  </si>
+  <si>
+    <t>countries_tnc_intersect.gpkg; pasture_equalarea.vrt</t>
+  </si>
+  <si>
+    <t>NLCD 2016 tabulated by each of the shapefiles; Historic 1700 landcover tabulated by each of the shapefiles; CDL tabulated by each of the shapefiles; rasterized TNC tabulated by CFS and by state; rasterized BCR tabulated by CFS and by state; global cropland  tabulated by intersected country x TNC</t>
+  </si>
+  <si>
+    <t>NLCD 2016 raster; historic 1700 land cover raster; CDL raster; rasterized TNC and BCR (Created elsewhere); global cropland rasters</t>
+  </si>
+  <si>
+    <t>Counts of pasture by country x ecoregion</t>
+  </si>
+  <si>
+    <t>raw_data/landuse/output_csvs/global_count_pasture.csv</t>
+  </si>
+  <si>
+    <t>spatial_processing/intersect_tnc_countries.R</t>
+  </si>
+  <si>
+    <t>Global TNC GPKG; Global countries GPKG</t>
+  </si>
+  <si>
+    <t>See output of transform_tnc_countries.sh</t>
+  </si>
+  <si>
+    <t>Intersected GPKG of TNC and countries</t>
+  </si>
+  <si>
+    <t>countries_tnc_intersect.gpkg</t>
+  </si>
+  <si>
+    <t>FAO/fao_transfers_by_ecoregion.R</t>
+  </si>
+  <si>
+    <t>intersected country boundaries x TNC GPKG; country GPKG; crop and pasture tabulated rasters; virtual land transfers into USA from countries</t>
+  </si>
+  <si>
+    <t>incoming VLT by country-TNC combination, and by 8 region-TNC combination, and land area from each foreign ecoregion in each of the 8 FAF rest of world regions</t>
+  </si>
+  <si>
+    <t>foreign_VLT_by_country_x_TNC.csv; foreign_VLT_by_region_x_TNC.csv; foreign_ecoregion_land_by_FAF.csv</t>
+  </si>
+  <si>
+    <t>countries_tnc_intersect.gpkg; raw_data/landuse/ecoregions/countries_global_equalarea.gpkg; raw_data/landuse/output_csvs/global_count_*.csv; foreign_VLT_by_country.csv</t>
+  </si>
+  <si>
+    <t>begins by sourcing faf_land_transfers.R, and additionally NLCD tabulated by the CFS-TNC intersect. As of 17 Sep., also takes some other inputs for calculating the foreign incoming transfers from ecoregions: the foreign VLTs from countries by TNC and land area per foreign FAF region for each TNC region</t>
+  </si>
+  <si>
+    <t>raw_data/landuse/output_csvs/NLCD_2016_CFSTNC.csv; foreign_VLT_by_country_x_TNC.csv; foreign_ecoregion_land_by_FAF.csv</t>
+  </si>
+  <si>
+    <t>Intermediate outputs: NLCD cropland and pastureland totals by CFS-TNC intersect; FAF by BEA object modified with all cropland and pastureland flows (and similar object for foreign flows); exiting flows of cropland and pastureland from TNC regions to FAF regions (and foreign regions). Additional outputs: TNC x TNC x FAF x FAF flows (all combinations) of land, and TNC x TNC aggregated flows (also similar outputs for foreign regions)</t>
+  </si>
+  <si>
+    <t>Domestic: NLCDcrop_FAF_x_TNC.csv; FAF_all_flows_x_BEA.csv; FAF_all_flows_x_TNC.csv; FAF_all_flows_TNC_x_TNC.csv; TNC_x_TNC_all_flows.csv. Foreign: FAF_foreign_flows_x_TNC.csv; FAF_all_foreign_flows_TNC_x_TNC.csv; TNC_x_TNC_all_foreign_flows.csv</t>
   </si>
 </sst>
 </file>
@@ -842,13 +902,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +950,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>
@@ -950,7 +1010,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>56</v>
@@ -985,7 +1045,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -993,124 +1053,124 @@
         <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1119,438 +1179,518 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>121</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update pipeline with scenario analysis shizz :hankey:
</commit_message>
<xml_diff>
--- a/pipelinetable.xlsx
+++ b/pipelinetable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="257">
   <si>
     <t>Path to script</t>
   </si>
@@ -458,18 +458,9 @@
     <t>cfs_io_analysis/faostat2017/*.csv; crossreference_tables/faostat_all_codes_harmonized.csv</t>
   </si>
   <si>
-    <t>virtual land transfers into USA from FAO trading partners for cropland and pastureland</t>
-  </si>
-  <si>
-    <t>fao_VLT_provisional.csv</t>
-  </si>
-  <si>
     <t>FAO/fao_vlt_by_fafregion.R</t>
   </si>
   <si>
-    <t>Lots of intermediate outputs are produced but currently not saved; some issues with output were resolved but still tagged provisional</t>
-  </si>
-  <si>
     <t>lookup table of FAF regions and UN regions, FAO virtual land transfers into USA by country</t>
   </si>
   <si>
@@ -569,15 +560,6 @@
     <t>begins by sourcing faf_land_transfers.R, and additionally NLCD tabulated by the CFS-TNC intersect. As of 17 Sep., also takes some other inputs for calculating the foreign incoming transfers from ecoregions: the foreign VLTs from countries by TNC and land area per foreign FAF region for each TNC region</t>
   </si>
   <si>
-    <t>raw_data/landuse/output_csvs/NLCD_2016_CFSTNC.csv; foreign_VLT_by_country_x_TNC.csv; foreign_ecoregion_land_by_FAF.csv</t>
-  </si>
-  <si>
-    <t>Intermediate outputs: NLCD cropland and pastureland totals by CFS-TNC intersect; FAF by BEA object modified with all cropland and pastureland flows (and similar object for foreign flows); exiting flows of cropland and pastureland from TNC regions to FAF regions (and foreign regions). Additional outputs: TNC x TNC x FAF x FAF flows (all combinations) of land, and TNC x TNC aggregated flows (also similar outputs for foreign regions)</t>
-  </si>
-  <si>
-    <t>Domestic: NLCDcrop_FAF_x_TNC.csv; FAF_all_flows_x_BEA.csv; FAF_all_flows_x_TNC.csv; FAF_all_flows_TNC_x_TNC.csv; TNC_x_TNC_all_flows.csv. Foreign: FAF_foreign_flows_x_TNC.csv; FAF_all_foreign_flows_TNC_x_TNC.csv; TNC_x_TNC_all_foreign_flows.csv</t>
-  </si>
-  <si>
     <t>none (intermediate, produces objects in R workspace); some are for data analysis while others are for mapping</t>
   </si>
   <si>
@@ -602,19 +584,217 @@
     <t>Scenario analysis</t>
   </si>
   <si>
-    <t>FAF/optimaltransport.R</t>
-  </si>
-  <si>
     <t>FAF by BEA CSV file; CFS Albers shapefile; BEA code lookup table</t>
   </si>
   <si>
     <t>Freight_Analysis_Framework_Regions/cfs_aea.gpkg; FAF_all_flows_x_BEA.csv; crossreference_tables/all_codes.csv</t>
   </si>
   <si>
-    <t>Optimal transport plans for each of the 10 BEA goods compared to observed plans; figures showing results</t>
-  </si>
-  <si>
-    <t>optimal_transport_results.Rdata; plots/optimal_transport*.png</t>
+    <t>Chaudhary/read_chaudh_si.R</t>
+  </si>
+  <si>
+    <t>raw supplemental table from Chaudhary 2015</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/xlsx file</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/chaudhary2015SI2.csv</t>
+  </si>
+  <si>
+    <t>moved from FWE repo</t>
+  </si>
+  <si>
+    <t>Chaudhary/prelim_biodiv_impacts.R</t>
+  </si>
+  <si>
+    <t>processed supplemental table of characterization factors (CFs)</t>
+  </si>
+  <si>
+    <t>baseline domestic and foreign TNC x TNC land flows (old version); CF data</t>
+  </si>
+  <si>
+    <t>TNC_x_TNC_all_flows.csv; TNC_x_TNC_all_foreign_flows.csv; biodiversity/chaudhary2015SI2.csv</t>
+  </si>
+  <si>
+    <t>Unfinished; Basically superseded by scenario_prelim_biodiv.R except for foreign flows</t>
+  </si>
+  <si>
+    <t>(not saved) domestic and foreign biodiversity flows, baseline only</t>
+  </si>
+  <si>
+    <t>FAO/extract_fbs.R</t>
+  </si>
+  <si>
+    <t>raw Food Balance Sheet data from FAOSTAT</t>
+  </si>
+  <si>
+    <t>raw_data/FAOSTAT/31aug2020/FoodBalanceSheets…</t>
+  </si>
+  <si>
+    <t>processed FBS</t>
+  </si>
+  <si>
+    <t>(none yet; unfinished)</t>
+  </si>
+  <si>
+    <t>production and trade totals for crops and animal products for the USA's trading partners; virtual land transfers into USA from FAO trading partners for cropland and pastureland</t>
+  </si>
+  <si>
+    <t>fao_production_trade_crops.csv; fao_production_trade_animals.csv; fao_VLT_provisional.csv</t>
+  </si>
+  <si>
+    <t>Some other intermediate outputs may not be saved; some issues with output were resolved but still tagged provisional</t>
+  </si>
+  <si>
+    <t>Misc data sources processing</t>
+  </si>
+  <si>
+    <t>scenario_analysis/lafa_calories_weight.R</t>
+  </si>
+  <si>
+    <t>sources script to load LAFA data from XLS sheets</t>
+  </si>
+  <si>
+    <t>read_lafa.R (in foodwasteinterventions repo)</t>
+  </si>
+  <si>
+    <t>calories by weight and total per capita calories for each LAFA item</t>
+  </si>
+  <si>
+    <t>lafa_calories_weight.csv</t>
+  </si>
+  <si>
+    <t>scenario_analysis/scenario_waste_reduction.R</t>
+  </si>
+  <si>
+    <t>FAF flows by BEA code (domestic and foreign), FAO production and trade data (foreign), FAO food loss and waste rates, waste rates by BEA code; BEA-FAO crosswalk</t>
+  </si>
+  <si>
+    <t>FAF_all_flows_x_BEA.csv; FAF_foreign_flows_x_BEA.csv; fao_production_trade_crops.csv; fao_production_trade_animals.csv; halvingfoodwaste/data/flw_rates.csv; crossreference_tables/waste_rates_bea.csv; crossreference_tables/naics_crosswalk_final.csv</t>
+  </si>
+  <si>
+    <t>scenarios/flows_wastereduced_domestic_provisional.csv</t>
+  </si>
+  <si>
+    <t>Only domestic is done so far (the foreign input data aren't used yet)</t>
+  </si>
+  <si>
+    <t>scenario_analysis/scenario_diet_shift.R</t>
+  </si>
+  <si>
+    <t>FAF flows by BEA code (domestic only); LAFA calories by weight</t>
+  </si>
+  <si>
+    <t>FAF_all_flows_x_BEA.csv; lafa_calories_weight.csv</t>
+  </si>
+  <si>
+    <t>scenarios/flows_dietshift_domestic_provisional.csv</t>
+  </si>
+  <si>
+    <t>Only domestic done so far</t>
+  </si>
+  <si>
+    <t>scenario_analysis/scenario_optimal_transport.R</t>
+  </si>
+  <si>
+    <t>scenarios/optimal_transport_results.Rdata; plots/optimal_transport*.png; scenarios/flows_optimaltransport_domestic_provisional.R</t>
+  </si>
+  <si>
+    <t>moved from FAF/optimaltransport.R; so far foreign flows are ignored, only domestic done</t>
+  </si>
+  <si>
+    <t>FAF/reduce_faf_data.R</t>
+  </si>
+  <si>
+    <t>large FAF by BEA Rdata file</t>
+  </si>
+  <si>
+    <t>faf_by_bea.Rdata</t>
+  </si>
+  <si>
+    <t>FAF flows for ag goods only in baseline scenario, both domestic+foreign and domestic only</t>
+  </si>
+  <si>
+    <t>scenarios/flows_baseline.csv; flows_baseline_domestic.csv</t>
+  </si>
+  <si>
+    <t>moved from scenarios folder</t>
+  </si>
+  <si>
+    <t>scenario_analysis/flows_to_land_transfers.R</t>
+  </si>
+  <si>
+    <t>Basically supersedes faf_land_transfers.R and faf_land_transfer_to_tnc.R, at least for domestic case (foreign not done yet)</t>
+  </si>
+  <si>
+    <t>Domestic VLT for each of the four scenarios, FAF lookup table (corrected), cropland and pastureland by FAF x TNC intersection, cropland and pastureland by state x FAF, population by FAF x TNC intersection</t>
+  </si>
+  <si>
+    <t>FAF shipments in the 50% waste reduction scenario</t>
+  </si>
+  <si>
+    <t>FAF shipments  in the 50% meat replacement scenario</t>
+  </si>
+  <si>
+    <t>Optimal transport plans for each of the 10 BEA goods compared to observed plans; figures showing results; FAF shipments in the optimal transport scenario</t>
+  </si>
+  <si>
+    <t>virtual land transfers for each of the 4 scenarios by FAF x FAF, FAF x TNC, and TNC x TNC, plus a summary total CSV</t>
+  </si>
+  <si>
+    <t>scenarios/landflows_allscenarios_provisional.csv; landflows_faf_tnc_x_tnc_scenarios_provisional.csv; landflows_tnc_x_tnc_scenarios_provisional.csv; landflows_totals_allscenarios_provisional.csv</t>
+  </si>
+  <si>
+    <t>scenarios/flows_*_domestic_provisional.csv (four); faf_region_lookup.csv; nass_bea_state_x_faf_land_totals.csv; NLCDcrop_FAF_x_TNC.csv; population_FAF_x_TNC_3column.csv</t>
+  </si>
+  <si>
+    <t>On 1 Oct, some intermediate outputs were moved from this script to others.</t>
+  </si>
+  <si>
+    <t>Intermediate outputs: NLCD cropland and pastureland totals by CFS-TNC intersect; exiting flows of cropland and pastureland from TNC regions to FAF regions (and foreign regions). Additional outputs: TNC x TNC x FAF x FAF flows (all combinations) of land, and TNC x TNC aggregated flows (also similar outputs for foreign regions)</t>
+  </si>
+  <si>
+    <t>Domestic:  FAF_all_flows_x_TNC.csv; FAF_all_flows_TNC_x_TNC.csv; TNC_x_TNC_all_flows.csv. Foreign: FAF_foreign_flows_x_TNC.csv; FAF_all_foreign_flows_TNC_x_TNC.csv; TNC_x_TNC_all_foreign_flows.csv</t>
+  </si>
+  <si>
+    <t>NLCDcrop_FAF_x_TNC.csv; foreign_VLT_by_country_x_TNC.csv; foreign_ecoregion_land_by_FAF.csv</t>
+  </si>
+  <si>
+    <t>spatial_processing/tabulate_nlcd_x_faf_x_tnc.R</t>
+  </si>
+  <si>
+    <t>raw output from shell script of NLCD by FAF x TNC</t>
+  </si>
+  <si>
+    <t>landuse/output_csvs/NLCD_2016_CFSTNC.csv</t>
+  </si>
+  <si>
+    <t>processed NLCD x FAF x TNC for the crop and pasture categories</t>
+  </si>
+  <si>
+    <t>NLCDcrop_FAF_x_TNC.csv</t>
+  </si>
+  <si>
+    <t>moved from FAF directory</t>
+  </si>
+  <si>
+    <t>scenario_analysis/scenario_prelim_biodiv.R</t>
+  </si>
+  <si>
+    <t>virtual land transfers TNC x TNC for each scenario; processed characterization factor data</t>
+  </si>
+  <si>
+    <t>scenarios/landflows_tnc_x_tnc_scenarios_provisional.csv; biodiversity/chaud2015SI2.csv</t>
+  </si>
+  <si>
+    <t>species lost by region for each scenario</t>
+  </si>
+  <si>
+    <t>scenarios/species_lost_scenarios_provisional.csv</t>
+  </si>
+  <si>
+    <t>BOTE AF</t>
   </si>
 </sst>
 </file>
@@ -935,13 +1115,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,13 +1266,13 @@
         <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -1103,19 +1283,19 @@
         <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1143,19 +1323,19 @@
         <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1163,47 +1343,50 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>247</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>248</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1212,559 +1395,783 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>226</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>227</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>229</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>230</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="270" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>155</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>186</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>187</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>189</v>
+        <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>97</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>193</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>237</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>196</v>
+        <v>216</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script to download cepii data
</commit_message>
<xml_diff>
--- a/pipelinetable.xlsx
+++ b/pipelinetable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="262">
   <si>
     <t>Path to script</t>
   </si>
@@ -795,6 +795,21 @@
   </si>
   <si>
     <t>BOTE AF</t>
+  </si>
+  <si>
+    <t>FAF/tabulate_annual_cropland.R</t>
+  </si>
+  <si>
+    <t>cropland and pastureland totals joined with FAF; NASS output with imputed data</t>
+  </si>
+  <si>
+    <t>NASS2012_receipts_workers_land_NAICS_imputed.csv; cropland_by_county_FAF_joined.csv</t>
+  </si>
+  <si>
+    <t>cropland and pastureland totals with FAF and with annual proportion</t>
+  </si>
+  <si>
+    <t>cropland_by_county_FAF_with_annual.csv</t>
   </si>
 </sst>
 </file>
@@ -1115,13 +1130,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,58 +1519,55 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>29</v>
@@ -1564,119 +1576,119 @@
         <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1684,265 +1696,265 @@
         <v>207</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>244</v>
+        <v>149</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>242</v>
+        <v>178</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>243</v>
+        <v>122</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>242</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1950,168 +1962,171 @@
         <v>185</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2119,58 +2134,78 @@
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update pipeline and remove unnecessary chaud scripts
</commit_message>
<xml_diff>
--- a/pipelinetable.xlsx
+++ b/pipelinetable.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="277">
   <si>
     <t>Path to script</t>
   </si>
@@ -815,9 +815,6 @@
     <t>scenarios/flows_2x2x2_factorial_domestic.csv; faf_region_lookup.csv; nass_bea_state_x_faf_land_totals.csv; NLCDcrop_FAF_x_TNC.csv; population_FAF_x_TNC_3column.csv</t>
   </si>
   <si>
-    <t>scenarios/landflows_tnc_x_tnc_2x2x2_factorial_provisional.csv; biodiversity/chaud2015SI2.csv</t>
-  </si>
-  <si>
     <t>scenarios/species_lost_2x2x2_factorial_provisional.csv</t>
   </si>
   <si>
@@ -840,6 +837,24 @@
   </si>
   <si>
     <t>Preliminary maps</t>
+  </si>
+  <si>
+    <t>Chaudhary/read_chaudh2018_si.R</t>
+  </si>
+  <si>
+    <t>raw supplemental table from Chaudhary 2018 (replaces 2015 data)</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/chaudhary_brooks_2018_si.xlsx</t>
+  </si>
+  <si>
+    <t>processed table of ecoregion summary info and of characterization factors (CFs)</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/chaud2018SI_ecoregions.csv and chaud2018SI_CFs.csv</t>
+  </si>
+  <si>
+    <t>scenarios/landflows_tnc_x_tnc_2x2x2_factorial_provisional.csv; biodiversity/chaud2018SI_CFs.csv</t>
   </si>
 </sst>
 </file>
@@ -1160,13 +1175,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,270 +1759,267 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>240</v>
+        <v>149</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>238</v>
+        <v>178</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>239</v>
+        <v>122</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>146</v>
+        <v>240</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>147</v>
+        <v>238</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -2015,191 +2027,194 @@
         <v>185</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>261</v>
+        <v>220</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2207,78 +2222,98 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>